<commit_message>
Modificações para o paper
</commit_message>
<xml_diff>
--- a/Conversão lat.xlsx
+++ b/Conversão lat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1DE5F9-1121-4180-8E59-970BEE2009A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D53CC9-65C9-4510-AD21-BBF2224D2538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="B1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Organizando os resultados das simulações para diferentes exoplanetas
</commit_message>
<xml_diff>
--- a/Conversão lat.xlsx
+++ b/Conversão lat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24272730-0DCA-4185-8D79-0C5022526DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4808E9E5-F905-4597-80B7-5C3F1723A92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="1095" windowWidth="18360" windowHeight="13545" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
+    <workbookView xWindow="18375" yWindow="705" windowWidth="18360" windowHeight="13545" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,7 +524,7 @@
   <dimension ref="B1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Simulações para 55 Cnc e
</commit_message>
<xml_diff>
--- a/Conversão lat.xlsx
+++ b/Conversão lat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DD2854-E2CA-4104-B88B-F19F978B6147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD5E3B8-189D-44EC-A1D4-2697A1AEB624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="16845" windowHeight="11325" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
+    <workbookView xWindow="19305" yWindow="1095" windowWidth="19155" windowHeight="13575" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -562,14 +562,14 @@
         <v>83.3</v>
       </c>
       <c r="C2" s="2">
-        <v>1.42</v>
+        <v>0.95</v>
       </c>
       <c r="D2" s="3">
-        <v>3.705E-2</v>
+        <v>1.5440000000000001E-2</v>
       </c>
       <c r="E2" s="1">
         <f>((1.496 * (10^8)) * D2) / (C2 * 696340)</f>
-        <v>5.60544529202385</v>
+        <v>3.4916760263815467</v>
       </c>
       <c r="F2">
         <f>PI()/180</f>
@@ -577,7 +577,7 @@
       </c>
       <c r="K2">
         <f>(ASIN(E2*COS(B2*F2))) / PI() * 180</f>
-        <v>40.843219310124923</v>
+        <v>24.040131545735598</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -602,26 +602,26 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2">
-        <v>1.42</v>
+        <v>0.95</v>
       </c>
       <c r="D5" s="3">
-        <v>3.705E-2</v>
+        <v>1.5440000000000001E-2</v>
       </c>
       <c r="E5">
         <f>(1.496 * (10^8)*D5) / (C5 * 696340)</f>
-        <v>5.60544529202385</v>
+        <v>3.4916760263815467</v>
       </c>
       <c r="K5">
         <f>180*(ACOS((SIN(B5*PI()/180))/E5)) / PI()</f>
-        <v>81.11236537954089</v>
+        <v>78.316099331953794</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K10">
-        <v>81.112365379540904</v>
+        <v>78.316099331953794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Novas simulações com GJ9827d
Fiz novas simulações com entradas de dados diferentes, como raio estelar menor obtido pelo artigo de 2023. Isso tem a finalidade de aumentar a profundidade de trânsito e diminuir a discrepância com os dados observacionais de WFC3
</commit_message>
<xml_diff>
--- a/Conversão lat.xlsx
+++ b/Conversão lat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4501394E-1731-4842-9159-B45FDAC67133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC777BD3-25C1-43EB-BC30-EA43DEE4E846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
+    <workbookView minimized="1" xWindow="17130" yWindow="1140" windowWidth="19155" windowHeight="13575" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -203,8 +203,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -524,7 +526,7 @@
   <dimension ref="B1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,18 +560,18 @@
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>87.442999999999998</v>
       </c>
       <c r="C2" s="2">
-        <v>0.60199999999999998</v>
+        <v>0.59940000000000004</v>
       </c>
       <c r="D2" s="3">
         <v>5.5899999999999998E-2</v>
       </c>
       <c r="E2" s="1">
         <f>((1.496 * (10^8)) * D2) / (C2 * 696340)</f>
-        <v>19.949203796175105</v>
+        <v>20.035736879041391</v>
       </c>
       <c r="F2">
         <f>PI()/180</f>
@@ -577,7 +579,7 @@
       </c>
       <c r="K2">
         <f>(ASIN(E2*COS(B2*F2))) / PI() * 180</f>
-        <v>62.873114240796639</v>
+        <v>63.362305668869112</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -601,27 +603,27 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
-        <v>30</v>
+      <c r="B5" s="4">
+        <v>50</v>
       </c>
       <c r="C5" s="2">
-        <v>0.60199999999999998</v>
+        <v>0.59940000000000004</v>
       </c>
       <c r="D5" s="3">
         <v>5.5899999999999998E-2</v>
       </c>
       <c r="E5">
         <f>(1.496 * (10^8)*D5) / (C5 * 696340)</f>
-        <v>19.949203796175105</v>
+        <v>20.035736879041391</v>
       </c>
       <c r="K5">
         <f>180*(ACOS((SIN(B5*PI()/180))/E5)) / PI()</f>
-        <v>88.563807845718131</v>
+        <v>87.80882458259488</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K10">
-        <v>88.563807845718102</v>
+        <v>87.808824582594895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustes finais antes da submissão do paper
</commit_message>
<xml_diff>
--- a/Conversão lat.xlsx
+++ b/Conversão lat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\StarsAndExoplanets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\Exoplanets\55Cnc_e\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE716F79-D361-4A59-A52C-6E649E0D2A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB76FAEC-DBB3-419A-9F91-0713562C04AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
+    <workbookView xWindow="15945" yWindow="810" windowWidth="19155" windowHeight="13575" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -61,7 +50,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -214,10 +203,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -537,20 +524,20 @@
   <dimension ref="B1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -570,19 +557,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="5">
-        <v>87.442999999999998</v>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="4">
+        <v>83.3</v>
       </c>
       <c r="C2" s="2">
-        <v>0.59940000000000004</v>
+        <v>0.95</v>
       </c>
       <c r="D2" s="3">
-        <v>5.5899999999999998E-2</v>
+        <v>1.5440000000000001E-2</v>
       </c>
       <c r="E2" s="1">
         <f>((1.496 * (10^8)) * D2) / (C2 * 696340)</f>
-        <v>20.035736879041391</v>
+        <v>3.4916760263815467</v>
       </c>
       <c r="F2">
         <f>PI()/180</f>
@@ -590,10 +577,10 @@
       </c>
       <c r="K2">
         <f>(ASIN(E2*COS(B2*F2))) / PI() * 180</f>
-        <v>63.362305668869112</v>
+        <v>24.040131545735598</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -613,28 +600,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="4">
-        <v>10</v>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
+        <v>45</v>
       </c>
       <c r="C5" s="2">
-        <v>0.59940000000000004</v>
+        <v>0.95</v>
       </c>
       <c r="D5" s="3">
-        <v>5.5899999999999998E-2</v>
+        <v>1.5440000000000001E-2</v>
       </c>
       <c r="E5">
         <f>(1.496 * (10^8)*D5) / (C5 * 696340)</f>
-        <v>20.035736879041391</v>
+        <v>3.4916760263815467</v>
       </c>
       <c r="K5">
         <f>180*(ACOS((SIN(B5*PI()/180))/E5)) / PI()</f>
-        <v>89.503415705512893</v>
+        <v>78.316099331953794</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K10">
-        <v>89.503415705512893</v>
+        <v>78.316099331953794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Facula to Simulations
</commit_message>
<xml_diff>
--- a/Conversão lat.xlsx
+++ b/Conversão lat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\Exoplanets\55Cnc_e\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\Exoplanets\GJ9827d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB76FAEC-DBB3-419A-9F91-0713562C04AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0832BAF0-22E9-4C73-A86F-34693F936AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15945" yWindow="810" windowWidth="19155" windowHeight="13575" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
+    <workbookView minimized="1" xWindow="2940" yWindow="3735" windowWidth="13785" windowHeight="11325" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,7 +524,7 @@
   <dimension ref="B1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,17 +559,17 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="4">
-        <v>83.3</v>
+        <v>87.442999999999998</v>
       </c>
       <c r="C2" s="2">
-        <v>0.95</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="D2" s="3">
-        <v>1.5440000000000001E-2</v>
+        <v>5.5899999999999998E-2</v>
       </c>
       <c r="E2" s="1">
         <f>((1.496 * (10^8)) * D2) / (C2 * 696340)</f>
-        <v>3.4916760263815467</v>
+        <v>19.949203796175105</v>
       </c>
       <c r="F2">
         <f>PI()/180</f>
@@ -577,7 +577,7 @@
       </c>
       <c r="K2">
         <f>(ASIN(E2*COS(B2*F2))) / PI() * 180</f>
-        <v>24.040131545735598</v>
+        <v>62.873114240796639</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -602,26 +602,26 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2">
-        <v>0.95</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="D5" s="3">
-        <v>1.5440000000000001E-2</v>
+        <v>5.5899999999999998E-2</v>
       </c>
       <c r="E5">
         <f>(1.496 * (10^8)*D5) / (C5 * 696340)</f>
-        <v>3.4916760263815467</v>
+        <v>19.949203796175105</v>
       </c>
       <c r="K5">
         <f>180*(ACOS((SIN(B5*PI()/180))/E5)) / PI()</f>
-        <v>78.316099331953794</v>
+        <v>89.01764145289971</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K10">
-        <v>78.316099331953794</v>
+        <v>89.017641452899696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Últimas simulações para o parâmetro de impacto
</commit_message>
<xml_diff>
--- a/Conversão lat.xlsx
+++ b/Conversão lat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\Exoplanets\GJ9827d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0832BAF0-22E9-4C73-A86F-34693F936AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD07465-A090-4829-BFAD-08C10568DC91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2940" yWindow="3735" windowWidth="13785" windowHeight="11325" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{F010B853-5C37-4295-ACFC-BAB654A3AB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,7 +524,7 @@
   <dimension ref="B1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,17 +559,17 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="4">
-        <v>87.442999999999998</v>
+        <v>79.569999999999993</v>
       </c>
       <c r="C2" s="2">
-        <v>0.60199999999999998</v>
+        <v>1.59</v>
       </c>
       <c r="D2" s="3">
-        <v>5.5899999999999998E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E2" s="1">
         <f>((1.496 * (10^8)) * D2) / (C2 * 696340)</f>
-        <v>19.949203796175105</v>
+        <v>5.134483028333408</v>
       </c>
       <c r="F2">
         <f>PI()/180</f>
@@ -577,7 +577,7 @@
       </c>
       <c r="K2">
         <f>(ASIN(E2*COS(B2*F2))) / PI() * 180</f>
-        <v>62.873114240796639</v>
+        <v>68.359587176773701</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>